<commit_message>
2013-2014 data acquisition fix
</commit_message>
<xml_diff>
--- a/metadata/STR-NHANES-2013-2014.xlsx
+++ b/metadata/STR-NHANES-2013-2014.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB095EA-3DB1-784A-BD44-9289F7E6A786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F960FE-7B19-5049-845B-3CEC0CE605B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20940" yWindow="-30020" windowWidth="24280" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1558,7 +1558,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>